<commit_message>
Normalise and validate MNO request phone numbers
This commit:

- switches phone number validation from a regexp to the 'phonelib' gem
- applies phone number normalisation (again using the same gem) prior to
saving the record
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/extra-mobile-data-requests.xlsx
+++ b/spec/fixtures/files/extra-mobile-data-requests.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Projects/dfe/get-help-with-tech/spec/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benilovj/workspace/dfe/get-help-with-tech/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B375B2DF-6308-0444-9DF5-BBBD2924D33C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC31F28D-6488-A840-8736-F556B7603D0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DWk/iI7WJL6C+29bLNvgmP9ozehQ9C9oeiDq1CRor61tRCfOkNhTAafC0gPhAS1sBd0CH8+wSoDIet5MQgj1pA==" workbookSaltValue="hAOPV+djOyk2S2VTK2Zbvw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="9440" yWindow="-19800" windowWidth="19160" windowHeight="10820" xr2:uid="{AA4C7391-D3C3-7D40-8CFA-8B3DBA3113B4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{AA4C7391-D3C3-7D40-8CFA-8B3DBA3113B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Extra mobile data requests" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>Felicity Hamburger</t>
   </si>
   <si>
-    <t>07000222222</t>
-  </si>
-  <si>
     <t>07111456789</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>07001234567</t>
+  </si>
+  <si>
+    <t>07900222222</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,7 +564,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -581,7 +581,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -598,7 +598,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -615,7 +615,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>

</xml_diff>